<commit_message>
Modify some diagrams according to final report.
</commit_message>
<xml_diff>
--- a/diagrams/API.xlsx
+++ b/diagrams/API.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\학교\소개원실\diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SNUPS\Desktop\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>POST</t>
   </si>
@@ -140,114 +140,134 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>About</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write new Question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write new Information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/auth/userinfo/:id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perform login and create session with backend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create new user account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get information about user with specific id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/posts/question/:id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Question object correspond to specific id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/list/tags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get every existing tags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/notifications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/newsfeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/newsfeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mark a newsfeed as read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get list of new notifications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get list of unread newsfeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/watchtags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setup a user's watch tag list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/api/vote/:id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Get list of votes with specific Information id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST</t>
+    <t>Add a vote to an Information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get votes corresponding to an Information</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>/api/vote</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apply new vote on the information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>URL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>About</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Write new Question</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Write new Information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/auth/userinfo/:id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Perform login and create session with backend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create new user account</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get information about user with specific id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DELETE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/posts/question/:id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Delete Question object correspond to specific id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/list/questions/type/:type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get list of Questions with specific type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/list/informations/type/:type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get list of Informations with specific type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/list/all/type/:type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get list of Questions and Informations with specific type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,7 +477,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -473,7 +493,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -737,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:K67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -752,13 +772,13 @@
   <sheetData>
     <row r="6" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -769,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -780,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -790,13 +810,13 @@
     </row>
     <row r="10" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -828,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -844,13 +864,13 @@
     </row>
     <row r="16" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -877,7 +897,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -887,13 +907,13 @@
     </row>
     <row r="21" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -920,40 +940,40 @@
     </row>
     <row r="24" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="5" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D27" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -961,133 +981,196 @@
         <v>10</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
+      <c r="D31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="5" t="s">
+      <c r="E33" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="6" t="s">
+    </row>
+    <row r="44" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="7" t="s">
+    </row>
+    <row r="45" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="4:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D38" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="F47" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="D49" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="D50" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -1098,7 +1181,7 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1109,7 +1192,7 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -1120,7 +1203,7 @@
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -1131,7 +1214,7 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -1142,7 +1225,7 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -1153,7 +1236,7 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -1164,18 +1247,15 @@
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -1186,7 +1266,7 @@
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>

</xml_diff>